<commit_message>
Some modification about the titles
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Armes</t>
   </si>
@@ -181,9 +181,6 @@
     <t>Poigne démoniaque</t>
   </si>
   <si>
-    <t>Etrange gant aspirant la vitalité de l'utilisateur pour le protéger lors d'un attaque</t>
-  </si>
-  <si>
     <t>(-15)% vie (perma)
 55 robustesse</t>
   </si>
@@ -214,13 +211,34 @@
   </si>
   <si>
     <t>7 atq physique</t>
+  </si>
+  <si>
+    <t>Dague</t>
+  </si>
+  <si>
+    <t>Bouclier</t>
+  </si>
+  <si>
+    <t>Épée</t>
+  </si>
+  <si>
+    <t>Armure
+casque</t>
+  </si>
+  <si>
+    <t>Armure
+jambière</t>
+  </si>
+  <si>
+    <t>Armure 
+corps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +249,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -269,17 +295,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -328,6 +345,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,400 +665,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="3">
         <v>25</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <v>5600</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="4">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="4">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>10</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="5">
         <v>70</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>8</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>430</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>835</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>12</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="4">
         <v>1525</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="4"/>
+    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>20</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>10</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="11" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>28</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>45</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="12" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>10</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>210</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="11" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7" t="s">
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>30</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>380</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="12" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>50</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>610</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <v>2</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="4">
         <v>4800</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4">
+        <v>4800</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="12" t="s">
+      <c r="H14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="12" t="s">
+    </row>
+    <row r="15" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="3">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="6">
-        <v>8</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="C17" s="4">
+        <v>16</v>
+      </c>
+      <c r="D17" s="4">
+        <v>100</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="3">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3">
+        <v>6500</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="4">
+        <v>30</v>
+      </c>
+      <c r="D19" s="4">
+        <v>6500</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3">
         <v>20</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="7">
-        <v>16</v>
-      </c>
-      <c r="D17" s="7">
-        <v>100</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="6">
-        <v>30</v>
-      </c>
-      <c r="D18" s="6">
-        <v>6500</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="7">
-        <v>30</v>
-      </c>
-      <c r="D19" s="7">
-        <v>6500</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="D20" s="3">
+        <v>350</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="6">
-        <v>20</v>
-      </c>
-      <c r="D20" s="6">
-        <v>350</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>15</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="4">
         <v>650</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>